<commit_message>
x(zone, zone) =1 means  -this zone is an entry  -we should place barriers on all its areas in contact with seawater the cost of those barriers is taken into account in the objective function.
</commit_message>
<xml_diff>
--- a/instance_1.xlsx
+++ b/instance_1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaae\PycharmProjects\SaveAssets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF6EFBA-527A-4967-8D23-BF70307BC64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19770" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
     <sheet name="Assets" sheetId="2" r:id="rId2"/>
     <sheet name="RegionLevel" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -45,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,11 +115,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -155,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +201,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,6 +253,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,14 +446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -419,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -427,7 +477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -441,14 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -459,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -470,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -481,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -498,14 +548,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>8</v>
       </c>
@@ -534,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -563,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>4</v>
       </c>
@@ -592,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>6</v>
       </c>
@@ -621,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -650,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9</v>
       </c>
@@ -679,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -708,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -737,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Try to apply the dual annealing
</commit_message>
<xml_diff>
--- a/instance_1.xlsx
+++ b/instance_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaae\PycharmProjects\SaveAssets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\assets_v_seawater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF6EFBA-527A-4967-8D23-BF70307BC64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B231E1F4-F44D-49FB-8C94-BD9DF99BB5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19770" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
@@ -451,9 +451,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -477,7 +477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -496,9 +496,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -549,273 +549,397 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="G6">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
         <v>4</v>
       </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>9</v>
       </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
         <v>9</v>
       </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
         <v>4</v>
       </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remarks& SA return numbers from 0 to 1
</commit_message>
<xml_diff>
--- a/instance_1.xlsx
+++ b/instance_1.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\assets_v_seawater\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B231E1F4-F44D-49FB-8C94-BD9DF99BB5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
     <sheet name="Assets" sheetId="2" r:id="rId2"/>
     <sheet name="RegionLevel" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,8 +45,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,19 +109,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -169,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,27 +187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,24 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,14 +396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -477,7 +427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -491,14 +441,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,7 +459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -520,7 +470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -531,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -548,398 +498,272 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1">
-        <v>3</v>
-      </c>
-      <c r="J1">
-        <v>3</v>
-      </c>
-      <c r="K1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>9</v>
       </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
       <c r="F8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remarks SA_return numbers from 0 to 1
</commit_message>
<xml_diff>
--- a/instance_1.xlsx
+++ b/instance_1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\assets_v_seawater\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A64C1-56F7-4FF2-836D-4EBEFFB808FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
     <sheet name="Assets" sheetId="2" r:id="rId2"/>
     <sheet name="RegionLevel" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -45,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,11 +115,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -155,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +201,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,6 +253,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,14 +446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -419,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -427,7 +477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -441,14 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -459,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -470,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -481,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -498,14 +548,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>8</v>
       </c>
@@ -534,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -563,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -592,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -621,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -650,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -679,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -708,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -737,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>

</xml_diff>